<commit_message>
add function to fill in blank serial numbers
</commit_message>
<xml_diff>
--- a/simple sheet test2.xlsx
+++ b/simple sheet test2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noelm\Documents\INF 360 Python\Create PDF's from 123\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A63D1F-8336-4DE2-BBB0-E0E1B583BABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C36003-324D-4E6D-8496-4047AE2A8368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{65BB431C-587B-49D6-B09F-D805D221EA00}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65BB431C-587B-49D6-B09F-D805D221EA00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
   <si>
     <t>LIN #</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Garmin GPS 601</t>
-  </si>
-  <si>
-    <t>58A022747</t>
   </si>
   <si>
     <t>58A022766</t>
@@ -558,7 +555,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,9 +614,7 @@
       <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="C4" s="9"/>
       <c r="D4" t="s">
         <v>7</v>
       </c>
@@ -632,18 +627,21 @@
         <v>9</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="36" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>

</xml_diff>